<commit_message>
aggiunti file di test. aggiornato foglio dei test.
</commit_message>
<xml_diff>
--- a/test-estrazione-dati/raccolta-test.xlsx
+++ b/test-estrazione-dati/raccolta-test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="122">
   <si>
     <t xml:space="preserve">Macchina</t>
   </si>
@@ -229,7 +229,58 @@
     <t xml:space="preserve">Qwen2.5:3b-instruct-fp16</t>
   </si>
   <si>
+    <t xml:space="preserve">6.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incoerente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.69</t>
+  </si>
+  <si>
     <t xml:space="preserve">Qwen2.5:3b-instruct-q4_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.49</t>
   </si>
   <si>
     <t xml:space="preserve">L4-ram32gb</t>
@@ -460,7 +511,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,6 +524,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,15 +536,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -505,23 +556,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -543,14 +582,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -653,9 +684,9 @@
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+      <selection pane="bottomLeft" activeCell="G73" activeCellId="0" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -677,7 +708,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -703,7 +734,7 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -712,7 +743,7 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="1" t="n">
@@ -726,7 +757,7 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -735,7 +766,7 @@
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -749,7 +780,7 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -758,13 +789,13 @@
       <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -784,7 +815,7 @@
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -807,7 +838,7 @@
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="1" t="n">
@@ -815,13 +846,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -879,7 +910,7 @@
       <c r="F9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -899,10 +930,10 @@
       <c r="E10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="11" t="s">
+      <c r="F10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -922,10 +953,10 @@
       <c r="E11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="11" t="s">
+      <c r="F11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -948,10 +979,10 @@
       <c r="E12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="F12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -974,10 +1005,10 @@
       <c r="E13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1027,187 +1058,187 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="13" t="s">
+    <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="13" t="n">
+      <c r="G16" s="11" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="17" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="15" t="s">
+    <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="13" t="s">
+      <c r="D17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="15" t="s">
+      <c r="F17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="15" t="s">
+      <c r="F18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="15" t="s">
+      <c r="F19" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="13" t="s">
+      <c r="D20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="15" t="s">
+      <c r="F20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="13" t="s">
+      <c r="D21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="15" t="s">
+      <c r="F21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="13" t="s">
+      <c r="D22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="F22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="13" t="s">
+      <c r="D23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="14" t="s">
+      <c r="F23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1218,7 +1249,7 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -1227,10 +1258,10 @@
       <c r="E24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="12" t="s">
+      <c r="F24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1241,7 +1272,7 @@
       <c r="B25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -1264,7 +1295,7 @@
       <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -1287,7 +1318,7 @@
       <c r="B27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -1310,7 +1341,7 @@
       <c r="B28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1333,7 +1364,7 @@
       <c r="B29" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -1356,7 +1387,7 @@
       <c r="B30" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -1379,7 +1410,7 @@
       <c r="B31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="9" t="s">
@@ -1395,934 +1426,952 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="15" t="s">
+    <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="13" t="s">
+      <c r="D32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="F32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="F33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="13" t="s">
+      <c r="D34" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="15" t="s">
+      <c r="F34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E35" s="13" t="s">
+      <c r="D35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="F35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="13" t="s">
+      <c r="D36" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="15" t="s">
+      <c r="F36" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="13" t="s">
+      <c r="D37" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="15" t="s">
+      <c r="F37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" s="13" t="s">
+      <c r="D38" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F38" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="15" t="s">
+      <c r="F38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" s="13" t="s">
+      <c r="D39" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="17" t="s">
+      <c r="F39" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="16" t="s">
+      <c r="D40" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G40" s="16" t="n">
+      <c r="G40" s="13" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="41" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="17" t="s">
+    <row r="41" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41" s="16" t="s">
+      <c r="D41" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G41" s="16" t="n">
+      <c r="G41" s="13" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="42" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="17" t="s">
+    <row r="42" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E42" s="16" t="s">
+      <c r="D42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G42" s="16" t="n">
+      <c r="G42" s="13" t="n">
         <v>56</v>
       </c>
     </row>
-    <row r="43" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="17" t="s">
+    <row r="43" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E43" s="16" t="s">
+      <c r="D43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="16" t="n">
+      <c r="G43" s="13" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="44" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="17" t="s">
+    <row r="44" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="16" t="s">
+      <c r="D44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="16" t="n">
+      <c r="G44" s="13" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="45" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="17" t="s">
+    <row r="45" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="16" t="s">
+      <c r="D45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G45" s="16" t="n">
+      <c r="G45" s="13" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="46" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="17" t="s">
+    <row r="46" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="16" t="s">
+      <c r="D46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G46" s="16" t="n">
+      <c r="G46" s="13" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="47" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="17" t="s">
+    <row r="47" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="16" t="s">
+      <c r="D47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="F47" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G47" s="16" t="n">
+      <c r="G47" s="13" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="48" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="19" t="s">
+    <row r="48" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G48" s="20" t="n">
+      <c r="G48" s="15" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="49" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="21" t="s">
+    <row r="49" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E49" s="18" t="s">
+      <c r="D49" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G49" s="20" t="n">
+      <c r="G49" s="15" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="50" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="21" t="s">
+    <row r="50" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E50" s="18" t="s">
+      <c r="D50" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F50" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G50" s="20" t="n">
+      <c r="G50" s="15" t="n">
         <v>68</v>
       </c>
     </row>
-    <row r="51" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="21" t="s">
+    <row r="51" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E51" s="18" t="s">
+      <c r="D51" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F51" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G51" s="20" t="n">
+      <c r="G51" s="15" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="52" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="21" t="s">
+    <row r="52" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E52" s="18" t="s">
+      <c r="D52" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F52" s="20" t="n">
+      <c r="F52" s="15" t="n">
         <v>12.85</v>
       </c>
-      <c r="G52" s="20" t="n">
+      <c r="G52" s="15" t="n">
         <v>95</v>
       </c>
     </row>
-    <row r="53" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="21" t="s">
+    <row r="53" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E53" s="18" t="s">
+      <c r="D53" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F53" s="20" t="s">
+      <c r="F53" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="G53" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C54" s="21" t="s">
+      <c r="G53" s="15" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E54" s="18" t="s">
+      <c r="D54" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G54" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="21" t="s">
+      <c r="G54" s="17" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E55" s="18" t="s">
+      <c r="D55" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="F55" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G55" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" s="22" t="s">
+      <c r="G55" s="17" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D56" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E56" s="16" t="s">
+      <c r="D56" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G56" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="22" t="s">
+      <c r="F56" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G56" s="13" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D57" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="16" t="s">
+      <c r="D57" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G57" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="22" t="s">
+      <c r="F57" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G57" s="13" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E58" s="16" t="s">
+      <c r="D58" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F58" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G58" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="22" t="s">
+      <c r="F58" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G58" s="13" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E59" s="16" t="s">
+      <c r="D59" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F59" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G59" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="22" t="s">
+      <c r="F59" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G59" s="13" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="16" t="s">
+      <c r="D60" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F60" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G60" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C61" s="22" t="s">
+      <c r="F60" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="13" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E61" s="16" t="s">
+      <c r="D61" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F61" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G61" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" s="22" t="s">
+      <c r="F61" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G61" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62" s="16" t="s">
+      <c r="D62" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F62" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G62" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C63" s="22" t="s">
+      <c r="F62" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G62" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" s="16" t="s">
+      <c r="D63" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F63" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G63" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" s="18" t="s">
+      <c r="F63" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G63" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G64" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="65" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C65" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E65" s="18" t="s">
+      <c r="F64" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" s="15" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F65" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G65" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E66" s="18" t="s">
+      <c r="F65" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G65" s="15" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F66" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G66" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="67" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E67" s="18" t="s">
+      <c r="F66" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G66" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="F67" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G67" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="68" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C68" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E68" s="18" t="s">
+    </row>
+    <row r="67" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G67" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E68" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F68" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G68" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="69" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C69" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E69" s="18" t="s">
+      <c r="F68" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G68" s="15" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F69" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G69" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B70" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C70" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E70" s="18" t="s">
+      <c r="F69" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G69" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F70" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G70" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C71" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E71" s="18" t="s">
+      <c r="F70" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G70" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E71" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F71" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G71" s="20" t="s">
-        <v>38</v>
+      <c r="F71" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G71" s="15" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="s">
-        <v>70</v>
+      <c r="A72" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2332,20 +2381,20 @@
         <v>18</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G72" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G72" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="s">
-        <v>70</v>
+      <c r="A73" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2355,20 +2404,20 @@
         <v>44</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="s">
-        <v>70</v>
+      <c r="A74" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2378,227 +2427,227 @@
         <v>44</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="s">
-        <v>70</v>
+      <c r="A75" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>75</v>
+        <v>91</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="G75" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7" t="s">
-        <v>70</v>
+      <c r="A76" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C76" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="G76" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="s">
-        <v>70</v>
+      <c r="A77" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C77" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F77" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G77" s="7" t="s">
-        <v>79</v>
+      <c r="F77" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7" t="s">
-        <v>70</v>
+      <c r="A78" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C78" s="24" t="s">
+      <c r="C78" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F78" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>82</v>
+      <c r="F78" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="s">
-        <v>70</v>
+      <c r="A79" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>84</v>
+      <c r="F79" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="G79" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="s">
-        <v>70</v>
+      <c r="A80" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C80" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F80" s="6" t="s">
-        <v>86</v>
+      <c r="F80" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="G80" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="s">
-        <v>70</v>
+      <c r="A81" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C81" s="24" t="s">
+      <c r="C81" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G81" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="7" t="s">
-        <v>70</v>
+      <c r="A82" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C82" s="24" t="s">
+      <c r="C82" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="7" t="s">
-        <v>70</v>
+      <c r="A83" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C84" s="25" t="s">
+      <c r="C84" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -2608,7 +2657,7 @@
         <v>18</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="G84" s="9" t="n">
         <v>80</v>
@@ -2616,12 +2665,12 @@
     </row>
     <row r="85" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C85" s="25" t="s">
+      <c r="C85" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D85" s="9" t="s">
@@ -2631,20 +2680,20 @@
         <v>45</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C86" s="25" t="s">
+      <c r="C86" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D86" s="9" t="s">
@@ -2654,89 +2703,89 @@
         <v>47</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G86" s="9" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="87" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B87" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C87" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E87" s="26" t="s">
+    <row r="87" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F87" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G87" s="26" t="n">
+      <c r="F87" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" s="21" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="88" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B88" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C88" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D88" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E88" s="26" t="s">
+    <row r="88" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E88" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F88" s="26" t="n">
+      <c r="F88" s="21" t="n">
         <v>20.24</v>
       </c>
-      <c r="G88" s="26" t="n">
+      <c r="G88" s="21" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="89" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B89" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C89" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E89" s="26" t="s">
+    <row r="89" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F89" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="G89" s="26" t="n">
+      <c r="F89" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G89" s="21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="90" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C90" s="25" t="s">
+      <c r="C90" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -2746,7 +2795,7 @@
         <v>18</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="G90" s="9" t="n">
         <v>80</v>
@@ -2754,12 +2803,12 @@
     </row>
     <row r="91" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C91" s="25" t="s">
+      <c r="C91" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D91" s="9" t="s">
@@ -2769,20 +2818,20 @@
         <v>45</v>
       </c>
       <c r="F91" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G91" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="92" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C92" s="25" t="s">
+      <c r="C92" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -2792,78 +2841,78 @@
         <v>47</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="G92" s="9" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="93" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B93" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D93" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E93" s="16" t="s">
+    <row r="93" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E93" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F93" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="G93" s="16" t="n">
+      <c r="F93" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G93" s="13" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="94" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C94" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E94" s="16" t="s">
+    <row r="94" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F94" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G94" s="16" t="n">
+      <c r="F94" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G94" s="13" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="95" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E95" s="16" t="s">
+    <row r="95" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E95" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F95" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="G95" s="16" t="n">
+      <c r="F95" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G95" s="13" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
aggiunti script bash per velocizzare i test. aggiornato foglio dei test.
</commit_message>
<xml_diff>
--- a/test-estrazione-dati/raccolta-test.xlsx
+++ b/test-estrazione-dati/raccolta-test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="149">
   <si>
     <t xml:space="preserve">Macchina</t>
   </si>
@@ -142,13 +142,10 @@
     <t xml:space="preserve">prompt8</t>
   </si>
   <si>
-    <t xml:space="preserve">screenshot</t>
-  </si>
-  <si>
     <t xml:space="preserve">prompt9</t>
   </si>
   <si>
-    <t xml:space="preserve">da fare</t>
+    <t xml:space="preserve">2:55.39</t>
   </si>
   <si>
     <t xml:space="preserve">prompt9 da 473/2024</t>
@@ -157,42 +154,120 @@
     <t xml:space="preserve">prompt10</t>
   </si>
   <si>
+    <t xml:space="preserve">5:08.78</t>
+  </si>
+  <si>
     <t xml:space="preserve">prompt10 da 589/2021</t>
   </si>
   <si>
     <t xml:space="preserve">62/2023</t>
   </si>
   <si>
+    <t xml:space="preserve">3:40.54</t>
+  </si>
+  <si>
     <t xml:space="preserve">473/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">2:00.75</t>
+    <t xml:space="preserve">4:01.89</t>
   </si>
   <si>
     <t xml:space="preserve">589/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">2:54.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:42.93</t>
+    <t xml:space="preserve">6:44.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.56</t>
   </si>
   <si>
     <t xml:space="preserve">Llama3.2:3b-instruct-fp16 </t>
   </si>
   <si>
+    <t xml:space="preserve">5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incoerente</t>
+  </si>
+  <si>
     <t xml:space="preserve">Llama3.2:3b-instruct-q4_0</t>
   </si>
   <si>
+    <t xml:space="preserve">14.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incoerente. Se non perdesse tempo a generare cose inutili potrebbe stare sotto i 5sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.28</t>
+  </si>
+  <si>
     <t xml:space="preserve">Qwen2.5:7b-instruct-fp16</t>
   </si>
   <si>
     <t xml:space="preserve">11.85</t>
   </si>
   <si>
-    <t xml:space="preserve">19.34</t>
-  </si>
-  <si>
     <t xml:space="preserve">48.34</t>
   </si>
   <si>
@@ -254,9 +329,6 @@
   </si>
   <si>
     <t xml:space="preserve">29.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incoerente</t>
   </si>
   <si>
     <t xml:space="preserve">31.47</t>
@@ -515,7 +587,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,6 +637,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,7 +762,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -929,8 +1009,8 @@
       <c r="F10" s="10" t="n">
         <v>0.00974791666666667</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>40</v>
+      <c r="G10" s="9" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,16 +1027,16 @@
         <v>35</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,13 +1053,13 @@
         <v>35</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>42</v>
+      <c r="G12" s="9" t="n">
+        <v>60</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>45</v>
@@ -1002,10 +1082,10 @@
         <v>46</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="G13" s="9" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,13 +1102,13 @@
         <v>35</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G14" s="9" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,10 +1125,10 @@
         <v>35</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="9" t="n">
         <v>90</v>
@@ -1071,7 +1151,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="11" t="n">
         <v>80</v>
@@ -1094,10 +1174,10 @@
         <v>37</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="G17" s="11" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,10 +1197,10 @@
         <v>39</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,13 +1217,13 @@
         <v>35</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>42</v>
+        <v>55</v>
+      </c>
+      <c r="G19" s="11" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,13 +1240,13 @@
         <v>35</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,10 +1266,10 @@
         <v>46</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>42</v>
+        <v>57</v>
+      </c>
+      <c r="G21" s="11" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,13 +1286,13 @@
         <v>35</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>42</v>
+        <v>58</v>
+      </c>
+      <c r="G22" s="13" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,13 +1309,13 @@
         <v>35</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="G23" s="13" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,7 +1326,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>35</v>
@@ -1255,10 +1335,10 @@
         <v>18</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>42</v>
+        <v>61</v>
+      </c>
+      <c r="G24" s="14" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="25" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,7 +1349,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>35</v>
@@ -1278,10 +1358,10 @@
         <v>37</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>42</v>
+        <v>62</v>
+      </c>
+      <c r="G25" s="14" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="26" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,7 +1372,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>35</v>
@@ -1301,10 +1381,10 @@
         <v>39</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>42</v>
+        <v>63</v>
+      </c>
+      <c r="G26" s="14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,19 +1395,19 @@
         <v>22</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>42</v>
+        <v>64</v>
+      </c>
+      <c r="G27" s="14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1338,19 +1418,19 @@
         <v>22</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>42</v>
+        <v>65</v>
+      </c>
+      <c r="G28" s="14" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="29" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,7 +1441,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>35</v>
@@ -1370,10 +1450,10 @@
         <v>46</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>42</v>
+        <v>66</v>
+      </c>
+      <c r="G29" s="14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,19 +1464,19 @@
         <v>22</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>42</v>
+        <v>67</v>
+      </c>
+      <c r="G30" s="14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,22 +1487,25 @@
         <v>22</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+      <c r="G31" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" s="11" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
         <v>29</v>
       </c>
@@ -1430,7 +1513,7 @@
         <v>22</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>35</v>
@@ -1439,10 +1522,13 @@
         <v>18</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>42</v>
+        <v>71</v>
+      </c>
+      <c r="G32" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,7 +1539,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>35</v>
@@ -1462,10 +1548,13 @@
         <v>37</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>42</v>
+        <v>73</v>
+      </c>
+      <c r="G33" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1565,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>35</v>
@@ -1485,10 +1574,13 @@
         <v>39</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>42</v>
+        <v>74</v>
+      </c>
+      <c r="G34" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="11" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1499,19 +1591,22 @@
         <v>22</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>42</v>
+        <v>75</v>
+      </c>
+      <c r="G35" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,19 +1617,22 @@
         <v>22</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>42</v>
+        <v>76</v>
+      </c>
+      <c r="G36" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,7 +1643,7 @@
         <v>22</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>35</v>
@@ -1554,10 +1652,13 @@
         <v>46</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>42</v>
+        <v>77</v>
+      </c>
+      <c r="G37" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1568,19 +1669,19 @@
         <v>22</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>42</v>
+        <v>78</v>
+      </c>
+      <c r="G38" s="13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,783 +1692,786 @@
         <v>22</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G40" s="13" t="n">
+      <c r="F40" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" s="15" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="41" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41" s="13" t="s">
+    <row r="41" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="15" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="15" t="n">
         <v>56</v>
       </c>
-      <c r="G41" s="13" t="n">
+    </row>
+    <row r="43" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G43" s="15" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="15" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="15" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" s="15" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="17" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G49" s="17" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G50" s="17" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="17" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="17" t="n">
+        <v>12.85</v>
+      </c>
+      <c r="G52" s="17" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G53" s="17" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G54" s="17" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G55" s="17" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" s="15" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" s="15" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="42" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E42" s="13" t="s">
+    <row r="58" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G42" s="13" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G43" s="13" t="n">
+      <c r="F58" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" s="15" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G59" s="15" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="44" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G44" s="13" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="13" t="s">
+    <row r="60" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G60" s="15" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F61" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G61" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G64" s="17" t="n">
         <v>60</v>
       </c>
-      <c r="G45" s="13" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G46" s="13" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G47" s="13" t="n">
+    </row>
+    <row r="65" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G65" s="17" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G66" s="17" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G68" s="17" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="48" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G48" s="15" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="G49" s="15" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G50" s="15" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G51" s="15" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F52" s="15" t="n">
-        <v>12.85</v>
-      </c>
-      <c r="G52" s="15" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="53" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E53" s="15" t="s">
+    <row r="69" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F53" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G53" s="15" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" s="15" t="s">
+      <c r="F69" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="G69" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G54" s="15" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G55" s="15" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F56" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G56" s="13" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G57" s="13" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G58" s="13" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="13" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" s="13" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F61" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G61" s="13" t="n">
+    </row>
+    <row r="70" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G70" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="H61" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F62" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G62" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H62" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G63" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H63" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G64" s="15" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G65" s="15" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F66" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G66" s="15" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F67" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G67" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H67" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C68" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G68" s="15" t="n">
+      <c r="H70" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E71" s="17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="69" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E69" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="G69" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H69" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="70" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C70" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F70" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G70" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H70" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="71" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C71" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E71" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G71" s="15" t="n">
+      <c r="F71" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G71" s="17" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C72" s="17" t="s">
+      <c r="C72" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2377,7 +2481,7 @@
         <v>18</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>26</v>
@@ -2385,12 +2489,12 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="C73" s="19" t="s">
         <v>30</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2400,20 +2504,20 @@
         <v>46</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C74" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2423,30 +2527,30 @@
         <v>46</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C75" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="G75" s="1" t="n">
         <v>0</v>
@@ -2454,22 +2558,22 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="G76" s="1" t="n">
         <v>100</v>
@@ -2477,68 +2581,68 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C79" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="G79" s="1" t="n">
         <v>0</v>
@@ -2546,22 +2650,22 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C80" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="G80" s="1" t="n">
         <v>0</v>
@@ -2569,22 +2673,22 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="C81" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="G81" s="1" t="n">
         <v>100</v>
@@ -2592,58 +2696,58 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C84" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -2653,7 +2757,7 @@
         <v>18</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="G84" s="9" t="n">
         <v>80</v>
@@ -2661,127 +2765,127 @@
     </row>
     <row r="85" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C85" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C86" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="G86" s="9" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="87" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B87" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C87" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D87" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E87" s="19" t="s">
+    <row r="87" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F87" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G87" s="19" t="n">
+      <c r="F87" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="G87" s="21" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="88" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E88" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F88" s="19" t="n">
+    <row r="88" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F88" s="21" t="n">
         <v>20.24</v>
       </c>
-      <c r="G88" s="19" t="n">
+      <c r="G88" s="21" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="89" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F89" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="G89" s="19" t="n">
+    <row r="89" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G89" s="21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="90" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C90" s="18" t="s">
+      <c r="C90" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -2791,7 +2895,7 @@
         <v>18</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="G90" s="9" t="n">
         <v>80</v>
@@ -2799,116 +2903,116 @@
     </row>
     <row r="91" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C91" s="18" t="s">
+      <c r="C91" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C92" s="18" t="s">
+      <c r="C92" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="G92" s="9" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="93" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E93" s="13" t="s">
+    <row r="93" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E93" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F93" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G93" s="13" t="n">
+      <c r="F93" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G93" s="15" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="94" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B94" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E94" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F94" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G94" s="13" t="n">
+    <row r="94" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E94" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G94" s="15" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="95" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B95" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F95" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="G95" s="13" t="n">
+    <row r="95" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G95" s="15" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>